<commit_message>
Finished results writing and conclusions
</commit_message>
<xml_diff>
--- a/experiments/notes-experiment.xlsx
+++ b/experiments/notes-experiment.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcimerman/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcimerman/Documents/master-thesis/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>